<commit_message>
Fix format of xlsx spreadsheet
Spreadsheet not readable by PsychoPy, spaces?
</commit_message>
<xml_diff>
--- a/exp/task-switching-replication-trialtypes-balanced.xlsx
+++ b/exp/task-switching-replication-trialtypes-balanced.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -25,79 +25,79 @@
     <t xml:space="preserve">trialNum</t>
   </si>
   <si>
-    <t xml:space="preserve"> switchTrialType</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> congruantTrialType</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cueType</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> shapeType</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> shapeColor</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cueFileName</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> stimuliFileName</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> correctAnswer</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> solid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> triangle</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> stimuli/solid-rectangle.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> stimuli/blue-triangle.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> noswitch</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> congruant</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> yellow</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> stimuli/yellow-triangle.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> switch</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dashed</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> stimuli/dashed-rectangle.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> incongruant</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> square</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> stimuli/yellow-square.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> stimuli/blue-square.png</t>
+    <t xml:space="preserve">switchTrialType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">congruantTrialType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cueType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shapeType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shapeColor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cueFileName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stimuliFileName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correctAnswer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dashed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">square</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yellow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stimuli/dashed-rectangle.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stimuli/yellow-square.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incongruant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triangle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stimuli/solid-rectangle.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stimuli/blue-triangle.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stimuli/blue-square.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noswitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">congruant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stimuli/yellow-triangle.png</t>
   </si>
 </sst>
 </file>
@@ -202,14 +202,14 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -281,19 +281,19 @@
         <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>1</v>
@@ -304,25 +304,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>2</v>
@@ -333,25 +333,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>2</v>
@@ -365,22 +365,22 @@
         <v>15</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>1</v>
@@ -391,25 +391,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>1</v>
@@ -420,28 +420,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,28 +449,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,25 +478,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>2</v>
@@ -507,13 +507,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>11</v>
@@ -522,7 +522,7 @@
         <v>12</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>14</v>
@@ -536,25 +536,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>1</v>
@@ -568,22 +568,22 @@
         <v>15</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>2</v>
@@ -594,25 +594,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>1</v>
@@ -623,25 +623,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>2</v>
@@ -652,28 +652,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>25</v>
       </c>
       <c r="I16" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -681,25 +681,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>1</v>
@@ -710,28 +710,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -739,28 +739,28 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="I19" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,25 +768,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>1</v>
@@ -803,22 +803,22 @@
         <v>16</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -826,25 +826,25 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>1</v>
@@ -855,25 +855,25 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>1</v>
@@ -884,28 +884,28 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H24" s="0" t="s">
         <v>25</v>
       </c>
       <c r="I24" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -913,28 +913,28 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G25" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="I25" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -945,10 +945,10 @@
         <v>15</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>11</v>
@@ -957,7 +957,7 @@
         <v>12</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>14</v>
@@ -971,28 +971,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I27" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1000,7 +1000,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>16</v>
@@ -1012,16 +1012,16 @@
         <v>11</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I28" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,28 +1029,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H29" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="I29" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1058,28 +1058,28 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I30" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1087,25 +1087,25 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>1</v>
@@ -1116,28 +1116,28 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I32" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,25 +1145,25 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>2</v>
@@ -1174,28 +1174,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I34" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1203,28 +1203,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C35" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="I35" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1232,16 +1232,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>12</v>
@@ -1253,7 +1253,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,28 +1261,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I37" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1290,28 +1290,28 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G38" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I38" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1322,25 +1322,25 @@
         <v>15</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I39" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1348,25 +1348,25 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>2</v>
@@ -1380,22 +1380,22 @@
         <v>15</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I41" s="0" t="n">
         <v>1</v>
@@ -1406,28 +1406,28 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="I42" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1435,25 +1435,25 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E43" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I43" s="0" t="n">
         <v>1</v>
@@ -1467,22 +1467,22 @@
         <v>15</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I44" s="0" t="n">
         <v>1</v>
@@ -1493,28 +1493,28 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E45" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I45" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1522,28 +1522,28 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E46" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I46" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,28 +1551,28 @@
         <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G47" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I47" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,25 +1580,25 @@
         <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I48" s="0" t="n">
         <v>1</v>
@@ -1609,16 +1609,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>12</v>
@@ -1627,7 +1627,7 @@
         <v>13</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I49" s="0" t="n">
         <v>1</v>
@@ -1638,7 +1638,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>16</v>
@@ -1650,16 +1650,16 @@
         <v>11</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G50" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I50" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>